<commit_message>
Merge changes from GitHub
</commit_message>
<xml_diff>
--- a/Arrival_rates.xlsx
+++ b/Arrival_rates.xlsx
@@ -1,25 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\charl\OneDrive\Documents\VU vakken\OBP\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00F0D4B6-5DAE-44EF-8BF7-3821C200BFD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1 - Arrival_rates" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet 1 - Arrival_rates" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
   <si>
     <t>High_Complex</t>
   </si>
   <si>
     <t>GRZ</t>
-  </si>
-  <si>
-    <t>Low_Compex</t>
   </si>
   <si>
     <t>Respite_Care</t>
@@ -51,32 +57,22 @@
   <si>
     <t>0.54</t>
   </si>
+  <si>
+    <t>Low_Complex</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <sz val="15"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="1"/>
+      <b/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
@@ -223,39 +219,39 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="10">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -266,27 +262,85 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffbdc0bf"/>
-      <rgbColor rgb="ffa5a5a5"/>
-      <rgbColor rgb="ff3f3f3f"/>
-      <rgbColor rgb="ffdbdbdb"/>
-      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFBDC0BF"/>
+      <rgbColor rgb="FFA5A5A5"/>
+      <rgbColor rgb="FF3F3F3F"/>
+      <rgbColor rgb="FFDBDBDB"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Blank">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Blank">
   <a:themeElements>
     <a:clrScheme name="Blank">
       <a:dk1>
@@ -488,7 +542,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -507,7 +561,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -537,7 +591,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -563,7 +617,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -589,7 +643,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -615,7 +669,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -641,7 +695,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -667,7 +721,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -693,7 +747,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -719,7 +773,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -745,7 +799,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -758,9 +812,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -777,7 +837,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -796,7 +856,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -822,7 +882,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -848,7 +908,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -874,7 +934,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -900,7 +960,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -926,7 +986,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -952,7 +1012,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -978,7 +1038,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1004,7 +1064,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1030,7 +1090,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1043,9 +1103,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1059,7 +1125,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1078,7 +1144,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1108,7 +1174,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1134,7 +1200,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1160,7 +1226,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1186,7 +1252,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1212,7 +1278,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1238,7 +1304,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1264,7 +1330,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1290,7 +1356,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1316,7 +1382,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1329,104 +1395,114 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.33333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.28515625" defaultRowHeight="19.899999999999999" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="20.3516" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6719" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.1719" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.1719" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.6719" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.35156" style="1" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="20.25" customHeight="1">
+    <row r="1" spans="1:5" ht="20.25" customHeight="1">
       <c r="A1" s="2"/>
-      <c r="B1" t="s" s="3">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s" s="3">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s" s="3">
+      <c r="D1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s" s="3">
+    </row>
+    <row r="2" spans="1:5" ht="20.25" customHeight="1">
+      <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
+      <c r="B2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" ht="20.25" customHeight="1">
-      <c r="A2" t="s" s="4">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s" s="5">
+    <row r="3" spans="1:5" ht="20.100000000000001" customHeight="1">
+      <c r="A3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s" s="6">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s" s="6">
+      <c r="D3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E2" t="s" s="6">
-        <v>7</v>
+      <c r="E3" s="9" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="3" ht="20.05" customHeight="1">
-      <c r="A3" t="s" s="7">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s" s="8">
+    <row r="4" spans="1:5" ht="20.100000000000001" customHeight="1">
+      <c r="A4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="E3" t="s" s="9">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" t="s" s="7">
+      <c r="B4" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B4" t="s" s="8">
+      <c r="C4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s" s="9">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="E4" t="s" s="9">
-        <v>6</v>
+      <c r="D4" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>